<commit_message>
Inserido a data no rodapé da página
</commit_message>
<xml_diff>
--- a/Escala - Copia.xlsx
+++ b/Escala - Copia.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="319" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="322" uniqueCount="95">
   <si>
     <t>PERÍODO:</t>
   </si>
@@ -292,13 +292,25 @@
   </si>
   <si>
     <t>RESERVAS:</t>
+  </si>
+  <si>
+    <t>* 3S SIN VAZ</t>
+  </si>
+  <si>
+    <t>* 3S SIN PEDROSO</t>
+  </si>
+  <si>
+    <t>* Entrada e saída de serviço deve ser VERMELHA</t>
+  </si>
+  <si>
+    <t>Escala Roxa deve ser Inserido nos quadrinhos diretamente.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="21">
+  <fonts count="22">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -450,6 +462,14 @@
       <color rgb="FFFF0000"/>
       <name val="Calibri"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -525,7 +545,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="46">
+  <cellXfs count="47">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -583,9 +603,6 @@
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="16" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -610,6 +627,12 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -926,14 +949,13 @@
   <dimension ref="A1:CG51"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E1" sqref="E1"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.28515625" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="10.7109375" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="26.28515625" style="7" bestFit="1" customWidth="1"/>
-    <col min="2" max="5" width="12.28515625" style="4" customWidth="1"/>
-    <col min="6" max="16384" width="12.28515625" style="4"/>
+    <col min="2" max="16384" width="10.7109375" style="4"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:20">
@@ -941,12 +963,20 @@
         <v>0</v>
       </c>
       <c r="B1" s="5">
-        <v>43739</v>
+        <v>43770</v>
       </c>
       <c r="C1" s="5">
-        <v>43769</v>
-      </c>
-      <c r="E1" s="27"/>
+        <v>43799</v>
+      </c>
+      <c r="E1" s="37" t="s">
+        <v>93</v>
+      </c>
+      <c r="J1" s="37" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="2" spans="1:20">
+      <c r="C2" s="38"/>
     </row>
     <row r="3" spans="1:20" s="14" customFormat="1" ht="15.75" customHeight="1">
       <c r="A3" s="8" t="s">
@@ -967,20 +997,35 @@
         <v>2</v>
       </c>
       <c r="B4" s="15">
-        <v>43744</v>
+        <v>44110</v>
       </c>
       <c r="C4" s="15">
-        <v>43752</v>
+        <v>44118</v>
       </c>
       <c r="D4" s="15">
-        <v>43760</v>
+        <v>44126</v>
       </c>
       <c r="E4" s="15">
-        <v>43768</v>
-      </c>
-      <c r="F4" s="28"/>
-      <c r="G4" s="28"/>
-      <c r="H4" s="28"/>
+        <v>44134</v>
+      </c>
+      <c r="F4" s="27">
+        <v>44188</v>
+      </c>
+      <c r="G4" s="27">
+        <v>44189</v>
+      </c>
+      <c r="H4" s="27">
+        <v>43824</v>
+      </c>
+      <c r="I4" s="27">
+        <v>43826</v>
+      </c>
+      <c r="J4" s="27">
+        <v>43801</v>
+      </c>
+      <c r="K4" s="15">
+        <v>43903</v>
+      </c>
     </row>
     <row r="5" spans="1:20" s="18" customFormat="1">
       <c r="A5" s="10" t="s">
@@ -996,14 +1041,14 @@
       <c r="C6" s="17"/>
       <c r="D6" s="17"/>
     </row>
-    <row r="7" spans="1:20" s="30" customFormat="1">
-      <c r="A7" s="30" t="s">
+    <row r="7" spans="1:20" s="29" customFormat="1">
+      <c r="A7" s="29" t="s">
         <v>4</v>
       </c>
-      <c r="B7" s="38" t="s">
+      <c r="B7" s="39" t="s">
         <v>5</v>
       </c>
-      <c r="C7" s="39"/>
+      <c r="C7" s="40"/>
     </row>
     <row r="8" spans="1:20">
       <c r="A8" s="11" t="s">
@@ -2046,7 +2091,7 @@
     </row>
     <row r="32" spans="1:85">
       <c r="A32" s="11" t="s">
-        <v>30</v>
+        <v>92</v>
       </c>
       <c r="B32" s="15">
         <v>43645</v>
@@ -2105,7 +2150,7 @@
         <v>32</v>
       </c>
       <c r="B34" s="15"/>
-      <c r="C34" s="29"/>
+      <c r="C34" s="28"/>
       <c r="D34" s="15"/>
       <c r="E34" s="15"/>
       <c r="F34" s="15"/>
@@ -2330,7 +2375,7 @@
     </row>
     <row r="40" spans="1:34">
       <c r="A40" s="11" t="s">
-        <v>38</v>
+        <v>91</v>
       </c>
       <c r="B40" s="15"/>
       <c r="C40" s="15"/>
@@ -2674,7 +2719,7 @@
     <mergeCell ref="B7:C7"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
-  <pageSetup paperSize="9" orientation="portrait"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -2683,15 +2728,14 @@
   <sheetPr codeName="Plan2"/>
   <dimension ref="A1:AC36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="E1" sqref="E1"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C35" sqref="C35"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="10.7109375" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="26.28515625" style="22" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="10.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="29" width="9.140625" style="1" customWidth="1"/>
+    <col min="1" max="1" width="24.5703125" style="22" bestFit="1" customWidth="1"/>
+    <col min="2" max="29" width="10.7109375" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="26.25" customHeight="1">
@@ -2700,66 +2744,66 @@
       </c>
     </row>
     <row r="2" spans="1:3">
-      <c r="A2" s="32" t="s">
+      <c r="A2" s="31" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="32">
+      <c r="B2" s="31">
         <v>43752</v>
       </c>
     </row>
     <row r="3" spans="1:3">
-      <c r="A3" s="32" t="s">
+      <c r="A3" s="31" t="s">
         <v>7</v>
       </c>
-      <c r="B3" s="32">
+      <c r="B3" s="31">
         <v>43765</v>
       </c>
     </row>
     <row r="4" spans="1:3">
-      <c r="A4" s="32" t="s">
+      <c r="A4" s="31" t="s">
         <v>8</v>
       </c>
-      <c r="B4" s="32">
+      <c r="B4" s="31">
         <v>43764</v>
       </c>
     </row>
     <row r="5" spans="1:3">
-      <c r="A5" s="32" t="s">
+      <c r="A5" s="31" t="s">
         <v>9</v>
       </c>
-      <c r="B5" s="32">
+      <c r="B5" s="31">
         <v>43758</v>
       </c>
     </row>
     <row r="6" spans="1:3">
-      <c r="A6" s="32" t="s">
+      <c r="A6" s="31" t="s">
         <v>10</v>
       </c>
-      <c r="B6" s="32">
+      <c r="B6" s="31">
         <v>43757</v>
       </c>
     </row>
     <row r="7" spans="1:3">
-      <c r="A7" s="32" t="s">
+      <c r="A7" s="31" t="s">
         <v>11</v>
       </c>
-      <c r="B7" s="32">
+      <c r="B7" s="31">
         <v>43751</v>
       </c>
     </row>
     <row r="8" spans="1:3">
-      <c r="A8" s="32" t="s">
+      <c r="A8" s="31" t="s">
         <v>12</v>
       </c>
-      <c r="B8" s="32">
+      <c r="B8" s="31">
         <v>43750</v>
       </c>
     </row>
     <row r="9" spans="1:3">
-      <c r="A9" s="32" t="s">
+      <c r="A9" s="31" t="s">
         <v>42</v>
       </c>
-      <c r="B9" s="32">
+      <c r="B9" s="31">
         <v>43744</v>
       </c>
       <c r="C9" s="1">
@@ -2767,235 +2811,239 @@
       </c>
     </row>
     <row r="10" spans="1:3">
-      <c r="A10" s="32" t="s">
+      <c r="A10" s="31" t="s">
         <v>14</v>
       </c>
-      <c r="B10" s="32">
+      <c r="B10" s="31">
         <v>43743</v>
       </c>
     </row>
     <row r="11" spans="1:3">
-      <c r="A11" s="32" t="s">
+      <c r="A11" s="31" t="s">
         <v>15</v>
       </c>
-      <c r="B11" s="32">
+      <c r="B11" s="31">
         <v>43737</v>
       </c>
     </row>
     <row r="12" spans="1:3">
-      <c r="A12" s="32" t="s">
+      <c r="A12" s="31" t="s">
         <v>16</v>
       </c>
-      <c r="B12" s="32">
+      <c r="B12" s="31">
         <v>43736</v>
       </c>
     </row>
     <row r="13" spans="1:3">
-      <c r="A13" s="32" t="s">
+      <c r="A13" s="31" t="s">
         <v>17</v>
       </c>
-      <c r="B13" s="32">
+      <c r="B13" s="31">
         <v>43729</v>
       </c>
     </row>
     <row r="14" spans="1:3">
-      <c r="A14" s="32" t="s">
+      <c r="A14" s="31" t="s">
         <v>18</v>
       </c>
-      <c r="B14" s="32">
+      <c r="B14" s="31">
         <v>43730</v>
       </c>
     </row>
     <row r="15" spans="1:3">
-      <c r="A15" s="32" t="s">
+      <c r="A15" s="31" t="s">
         <v>19</v>
       </c>
-      <c r="B15" s="32">
+      <c r="B15" s="31">
         <v>43723</v>
       </c>
     </row>
     <row r="16" spans="1:3">
-      <c r="A16" s="32" t="s">
+      <c r="A16" s="31" t="s">
         <v>20</v>
       </c>
-      <c r="B16" s="32">
+      <c r="B16" s="31">
         <v>43722</v>
       </c>
     </row>
     <row r="17" spans="1:3">
-      <c r="A17" s="32" t="s">
+      <c r="A17" s="31" t="s">
         <v>21</v>
       </c>
-      <c r="B17" s="32">
+      <c r="B17" s="31">
         <v>43716</v>
       </c>
     </row>
     <row r="18" spans="1:3">
-      <c r="A18" s="32" t="s">
+      <c r="A18" s="31" t="s">
         <v>22</v>
       </c>
-      <c r="B18" s="32">
+      <c r="B18" s="31">
         <v>43715</v>
       </c>
     </row>
     <row r="19" spans="1:3">
-      <c r="A19" s="32" t="s">
+      <c r="A19" s="31" t="s">
         <v>23</v>
       </c>
-      <c r="B19" s="32">
+      <c r="B19" s="31">
         <v>43624</v>
       </c>
-      <c r="C19" s="32">
+      <c r="C19" s="31">
         <v>43631</v>
       </c>
     </row>
     <row r="20" spans="1:3">
-      <c r="A20" s="32" t="s">
+      <c r="A20" s="31" t="s">
         <v>24</v>
       </c>
-      <c r="B20" s="32">
+      <c r="B20" s="31">
         <v>43674</v>
       </c>
     </row>
     <row r="21" spans="1:3">
-      <c r="A21" s="32" t="s">
+      <c r="A21" s="31" t="s">
         <v>25</v>
       </c>
-      <c r="B21" s="32">
+      <c r="B21" s="31">
         <v>43709</v>
       </c>
     </row>
     <row r="22" spans="1:3">
-      <c r="A22" s="32" t="s">
+      <c r="A22" s="31" t="s">
         <v>26</v>
       </c>
-      <c r="B22" s="32">
+      <c r="B22" s="31">
         <v>43673</v>
       </c>
     </row>
     <row r="23" spans="1:3">
-      <c r="A23" s="32" t="s">
+      <c r="A23" s="31" t="s">
         <v>27</v>
       </c>
-      <c r="B23" s="32">
+      <c r="B23" s="31">
         <v>43667</v>
       </c>
     </row>
     <row r="24" spans="1:3">
-      <c r="A24" s="32" t="s">
+      <c r="A24" s="31" t="s">
         <v>28</v>
       </c>
-      <c r="B24" s="32">
+      <c r="B24" s="31">
         <v>43666</v>
       </c>
     </row>
     <row r="25" spans="1:3">
-      <c r="A25" s="32" t="s">
+      <c r="A25" s="31" t="s">
         <v>29</v>
       </c>
-      <c r="B25" s="32">
+      <c r="B25" s="31">
         <v>43660</v>
       </c>
-      <c r="C25" s="32">
+      <c r="C25" s="31">
         <v>43699</v>
       </c>
     </row>
     <row r="26" spans="1:3">
-      <c r="A26" s="32" t="s">
+      <c r="A26" s="31" t="s">
         <v>30</v>
       </c>
-      <c r="B26" s="32">
+      <c r="B26" s="31">
         <v>43653</v>
       </c>
     </row>
     <row r="27" spans="1:3">
-      <c r="A27" s="32" t="s">
+      <c r="A27" s="31" t="s">
         <v>31</v>
       </c>
-      <c r="B27" s="32">
+      <c r="B27" s="31">
         <v>43608</v>
       </c>
     </row>
     <row r="28" spans="1:3">
-      <c r="A28" s="32" t="s">
+      <c r="A28" s="31" t="s">
         <v>32</v>
       </c>
-      <c r="B28" s="32">
+      <c r="B28" s="31">
         <v>43607</v>
       </c>
     </row>
     <row r="29" spans="1:3">
-      <c r="A29" s="32" t="s">
+      <c r="A29" s="31" t="s">
         <v>33</v>
       </c>
-      <c r="B29" s="32">
+      <c r="B29" s="31">
         <v>43615</v>
       </c>
     </row>
     <row r="30" spans="1:3">
-      <c r="A30" s="32" t="s">
+      <c r="A30" s="31" t="s">
         <v>34</v>
       </c>
-      <c r="B30" s="32">
+      <c r="B30" s="31">
         <v>43614</v>
       </c>
     </row>
     <row r="31" spans="1:3">
-      <c r="A31" s="32" t="s">
+      <c r="A31" s="31" t="s">
         <v>35</v>
       </c>
-      <c r="B31" s="32">
+      <c r="B31" s="31">
         <v>43601</v>
       </c>
     </row>
     <row r="32" spans="1:3">
-      <c r="A32" s="32" t="s">
+      <c r="A32" s="31" t="s">
         <v>36</v>
       </c>
-      <c r="B32" s="32">
+      <c r="B32" s="31">
         <v>43652</v>
       </c>
     </row>
     <row r="33" spans="1:3">
-      <c r="A33" s="32" t="s">
+      <c r="A33" s="31" t="s">
         <v>37</v>
       </c>
-      <c r="B33" s="32" t="s">
+      <c r="B33" s="31" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="34" spans="1:3">
-      <c r="A34" s="32" t="s">
+      <c r="A34" s="31" t="s">
         <v>38</v>
       </c>
-      <c r="B34" s="32" t="s">
+      <c r="B34" s="31" t="s">
         <v>43</v>
       </c>
+      <c r="C34" s="1" t="s">
+        <v>43</v>
+      </c>
     </row>
     <row r="35" spans="1:3">
-      <c r="A35" s="32" t="s">
+      <c r="A35" s="31" t="s">
         <v>39</v>
       </c>
-      <c r="B35" s="32" t="s">
+      <c r="B35" s="31" t="s">
         <v>43</v>
       </c>
-      <c r="C35" s="32">
+      <c r="C35" s="31">
         <v>43768</v>
       </c>
     </row>
     <row r="36" spans="1:3">
-      <c r="A36" s="32" t="s">
+      <c r="A36" s="31" t="s">
         <v>40</v>
       </c>
-      <c r="B36" s="32">
+      <c r="B36" s="31">
         <v>43659</v>
       </c>
-      <c r="C36" s="32">
+      <c r="C36" s="31">
         <v>43760</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -3004,17 +3052,13 @@
   <sheetPr codeName="Plan3"/>
   <dimension ref="A1:AC36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="E1" sqref="E1"/>
-    </sheetView>
+    <sheetView topLeftCell="A4" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="10.7109375" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="26.28515625" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="10.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="29" width="9.140625" style="1" customWidth="1"/>
-    <col min="30" max="33" width="9.140625" style="31" customWidth="1"/>
-    <col min="34" max="16384" width="9.140625" style="31"/>
+    <col min="1" max="1" width="24.5703125" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="29" width="10.7109375" style="1"/>
+    <col min="30" max="16384" width="10.7109375" style="30"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="26.25" customHeight="1">
@@ -3023,342 +3067,342 @@
       </c>
     </row>
     <row r="2" spans="1:2">
-      <c r="A2" s="32" t="s">
+      <c r="A2" s="31" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="32">
+      <c r="B2" s="31">
         <v>43454</v>
       </c>
     </row>
     <row r="3" spans="1:2">
-      <c r="A3" s="32" t="s">
+      <c r="A3" s="31" t="s">
         <v>7</v>
       </c>
-      <c r="B3" s="32">
+      <c r="B3" s="31">
         <v>43734</v>
       </c>
     </row>
     <row r="4" spans="1:2">
-      <c r="A4" s="32" t="s">
+      <c r="A4" s="31" t="s">
         <v>8</v>
       </c>
-      <c r="B4" s="32">
+      <c r="B4" s="31">
         <v>43732</v>
       </c>
     </row>
     <row r="5" spans="1:2">
-      <c r="A5" s="32" t="s">
+      <c r="A5" s="31" t="s">
         <v>9</v>
       </c>
-      <c r="B5" s="32">
+      <c r="B5" s="31">
         <v>43731</v>
       </c>
     </row>
     <row r="6" spans="1:2">
-      <c r="A6" s="32" t="s">
+      <c r="A6" s="31" t="s">
         <v>10</v>
       </c>
-      <c r="B6" s="32">
+      <c r="B6" s="31">
         <v>43727</v>
       </c>
     </row>
     <row r="7" spans="1:2">
-      <c r="A7" s="32" t="s">
+      <c r="A7" s="31" t="s">
         <v>11</v>
       </c>
-      <c r="B7" s="32">
+      <c r="B7" s="31">
         <v>43726</v>
       </c>
     </row>
     <row r="8" spans="1:2">
-      <c r="A8" s="32" t="s">
+      <c r="A8" s="31" t="s">
         <v>12</v>
       </c>
-      <c r="B8" s="32">
+      <c r="B8" s="31">
         <v>43725</v>
       </c>
     </row>
     <row r="9" spans="1:2">
-      <c r="A9" s="32" t="s">
+      <c r="A9" s="31" t="s">
         <v>42</v>
       </c>
-      <c r="B9" s="32">
+      <c r="B9" s="31">
         <v>43724</v>
       </c>
     </row>
     <row r="10" spans="1:2">
-      <c r="A10" s="32" t="s">
+      <c r="A10" s="31" t="s">
         <v>14</v>
       </c>
-      <c r="B10" s="32">
+      <c r="B10" s="31">
         <v>43720</v>
       </c>
     </row>
     <row r="11" spans="1:2">
-      <c r="A11" s="32" t="s">
+      <c r="A11" s="31" t="s">
         <v>15</v>
       </c>
-      <c r="B11" s="32">
+      <c r="B11" s="31">
         <v>43719</v>
       </c>
     </row>
     <row r="12" spans="1:2">
-      <c r="A12" s="32" t="s">
+      <c r="A12" s="31" t="s">
         <v>16</v>
       </c>
-      <c r="B12" s="32">
+      <c r="B12" s="31">
         <v>43718</v>
       </c>
     </row>
     <row r="13" spans="1:2">
-      <c r="A13" s="32" t="s">
+      <c r="A13" s="31" t="s">
         <v>17</v>
       </c>
-      <c r="B13" s="32">
+      <c r="B13" s="31">
         <v>43717</v>
       </c>
     </row>
     <row r="14" spans="1:2">
-      <c r="A14" s="32" t="s">
+      <c r="A14" s="31" t="s">
         <v>18</v>
       </c>
-      <c r="B14" s="32">
+      <c r="B14" s="31">
         <v>43733</v>
       </c>
     </row>
     <row r="15" spans="1:2">
-      <c r="A15" s="32" t="s">
+      <c r="A15" s="31" t="s">
         <v>19</v>
       </c>
-      <c r="B15" s="32">
+      <c r="B15" s="31">
         <v>43713</v>
       </c>
     </row>
     <row r="16" spans="1:2">
-      <c r="A16" s="32" t="s">
+      <c r="A16" s="31" t="s">
         <v>20</v>
       </c>
-      <c r="B16" s="32">
+      <c r="B16" s="31">
         <v>43711</v>
       </c>
     </row>
     <row r="17" spans="1:3">
-      <c r="A17" s="32" t="s">
+      <c r="A17" s="31" t="s">
         <v>21</v>
       </c>
-      <c r="B17" s="32">
+      <c r="B17" s="31">
         <v>43710</v>
       </c>
-      <c r="C17" s="32">
+      <c r="C17" s="31">
         <v>43769</v>
       </c>
     </row>
     <row r="18" spans="1:3">
-      <c r="A18" s="32" t="s">
+      <c r="A18" s="31" t="s">
         <v>22</v>
       </c>
-      <c r="B18" s="32">
+      <c r="B18" s="31">
         <v>43676</v>
       </c>
-      <c r="C18" s="32">
+      <c r="C18" s="31">
         <v>43768</v>
       </c>
     </row>
     <row r="19" spans="1:3">
-      <c r="A19" s="32" t="s">
+      <c r="A19" s="31" t="s">
         <v>23</v>
       </c>
-      <c r="B19" s="32">
+      <c r="B19" s="31">
         <v>43675</v>
       </c>
-      <c r="C19" s="32">
+      <c r="C19" s="31">
         <v>43767</v>
       </c>
     </row>
     <row r="20" spans="1:3">
-      <c r="A20" s="32" t="s">
+      <c r="A20" s="31" t="s">
         <v>24</v>
       </c>
-      <c r="B20" s="32">
+      <c r="B20" s="31">
         <v>43671</v>
       </c>
-      <c r="C20" s="32">
+      <c r="C20" s="31">
         <v>43766</v>
       </c>
     </row>
     <row r="21" spans="1:3">
-      <c r="A21" s="32" t="s">
+      <c r="A21" s="31" t="s">
         <v>25</v>
       </c>
-      <c r="B21" s="32">
+      <c r="B21" s="31">
         <v>43712</v>
       </c>
-      <c r="C21" s="32">
+      <c r="C21" s="31">
         <v>43762</v>
       </c>
     </row>
     <row r="22" spans="1:3">
-      <c r="A22" s="32" t="s">
+      <c r="A22" s="31" t="s">
         <v>26</v>
       </c>
-      <c r="B22" s="32">
+      <c r="B22" s="31">
         <v>43668</v>
       </c>
-      <c r="C22" s="32">
+      <c r="C22" s="31">
         <v>43761</v>
       </c>
     </row>
     <row r="23" spans="1:3">
-      <c r="A23" s="32" t="s">
+      <c r="A23" s="31" t="s">
         <v>27</v>
       </c>
-      <c r="B23" s="32">
+      <c r="B23" s="31">
         <v>43670</v>
       </c>
-      <c r="C23" s="32">
+      <c r="C23" s="31">
         <v>43760</v>
       </c>
     </row>
     <row r="24" spans="1:3">
-      <c r="A24" s="32" t="s">
+      <c r="A24" s="31" t="s">
         <v>28</v>
       </c>
-      <c r="B24" s="32">
+      <c r="B24" s="31">
         <v>43669</v>
       </c>
-      <c r="C24" s="32">
+      <c r="C24" s="31">
         <v>43755</v>
       </c>
     </row>
     <row r="25" spans="1:3">
-      <c r="A25" s="32" t="s">
+      <c r="A25" s="31" t="s">
         <v>29</v>
       </c>
-      <c r="B25" s="32">
+      <c r="B25" s="31">
         <v>43664</v>
       </c>
-      <c r="C25" s="32">
+      <c r="C25" s="31">
         <v>43754</v>
       </c>
     </row>
     <row r="26" spans="1:3">
-      <c r="A26" s="32" t="s">
+      <c r="A26" s="31" t="s">
         <v>30</v>
       </c>
-      <c r="B26" s="32">
+      <c r="B26" s="31">
         <v>43663</v>
       </c>
-      <c r="C26" s="32">
+      <c r="C26" s="31">
         <v>43759</v>
       </c>
     </row>
     <row r="27" spans="1:3">
-      <c r="A27" s="32" t="s">
+      <c r="A27" s="31" t="s">
         <v>31</v>
       </c>
-      <c r="B27" s="32">
+      <c r="B27" s="31">
         <v>43662</v>
       </c>
-      <c r="C27" s="32">
+      <c r="C27" s="31">
         <v>43753</v>
       </c>
     </row>
     <row r="28" spans="1:3">
-      <c r="A28" s="32" t="s">
+      <c r="A28" s="31" t="s">
         <v>32</v>
       </c>
-      <c r="B28" s="32">
+      <c r="B28" s="31">
         <v>43661</v>
       </c>
-      <c r="C28" s="32">
+      <c r="C28" s="31">
         <v>43752</v>
       </c>
     </row>
     <row r="29" spans="1:3">
-      <c r="A29" s="32" t="s">
+      <c r="A29" s="31" t="s">
         <v>33</v>
       </c>
-      <c r="B29" s="32">
+      <c r="B29" s="31">
         <v>43657</v>
       </c>
-      <c r="C29" s="32">
+      <c r="C29" s="31">
         <v>43748</v>
       </c>
     </row>
     <row r="30" spans="1:3">
-      <c r="A30" s="32" t="s">
+      <c r="A30" s="31" t="s">
         <v>34</v>
       </c>
-      <c r="B30" s="32">
+      <c r="B30" s="31">
         <v>43656</v>
       </c>
-      <c r="C30" s="32">
+      <c r="C30" s="31">
         <v>43747</v>
       </c>
     </row>
     <row r="31" spans="1:3">
-      <c r="A31" s="32" t="s">
+      <c r="A31" s="31" t="s">
         <v>35</v>
       </c>
-      <c r="B31" s="32">
+      <c r="B31" s="31">
         <v>43650</v>
       </c>
-      <c r="C31" s="32">
+      <c r="C31" s="31">
         <v>43746</v>
       </c>
     </row>
     <row r="32" spans="1:3">
-      <c r="A32" s="32" t="s">
+      <c r="A32" s="31" t="s">
         <v>36</v>
       </c>
-      <c r="B32" s="32">
+      <c r="B32" s="31">
         <v>43655</v>
       </c>
-      <c r="C32" s="32">
+      <c r="C32" s="31">
         <v>43745</v>
       </c>
     </row>
     <row r="33" spans="1:3">
-      <c r="A33" s="32" t="s">
+      <c r="A33" s="31" t="s">
         <v>37</v>
       </c>
-      <c r="B33" s="32">
+      <c r="B33" s="31">
         <v>43649</v>
       </c>
-      <c r="C33" s="32">
+      <c r="C33" s="31">
         <v>43741</v>
       </c>
     </row>
     <row r="34" spans="1:3">
-      <c r="A34" s="32" t="s">
+      <c r="A34" s="31" t="s">
         <v>38</v>
       </c>
-      <c r="B34" s="32">
+      <c r="B34" s="31">
         <v>43648</v>
       </c>
-      <c r="C34" s="32">
+      <c r="C34" s="31">
         <v>43740</v>
       </c>
     </row>
     <row r="35" spans="1:3">
-      <c r="A35" s="32" t="s">
+      <c r="A35" s="31" t="s">
         <v>39</v>
       </c>
-      <c r="B35" s="32">
+      <c r="B35" s="31">
         <v>43647</v>
       </c>
-      <c r="C35" s="32">
+      <c r="C35" s="31">
         <v>43739</v>
       </c>
     </row>
     <row r="36" spans="1:3">
-      <c r="A36" s="32" t="s">
+      <c r="A36" s="31" t="s">
         <v>40</v>
       </c>
-      <c r="B36" s="32">
+      <c r="B36" s="31">
         <v>43654</v>
       </c>
-      <c r="C36" s="32">
+      <c r="C36" s="31">
         <v>43738</v>
       </c>
     </row>
@@ -3372,17 +3416,13 @@
   <sheetPr codeName="Plan4"/>
   <dimension ref="A1:AC36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="E1" sqref="E1"/>
-    </sheetView>
+    <sheetView topLeftCell="A16" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="10.7109375" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="26.28515625" style="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="29" width="9.140625" style="1" customWidth="1"/>
-    <col min="30" max="33" width="9.140625" style="31" customWidth="1"/>
-    <col min="34" max="16384" width="9.140625" style="31"/>
+    <col min="1" max="1" width="24.5703125" style="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="29" width="10.7109375" style="1"/>
+    <col min="30" max="16384" width="10.7109375" style="30"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1" ht="26.25" customHeight="1">
@@ -3391,213 +3431,213 @@
       </c>
     </row>
     <row r="2" spans="1:1">
-      <c r="A2" s="32" t="s">
+      <c r="A2" s="31" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="3" spans="1:1">
-      <c r="A3" s="32" t="s">
+      <c r="A3" s="31" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="4" spans="1:1">
-      <c r="A4" s="32" t="s">
+      <c r="A4" s="31" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="5" spans="1:1">
-      <c r="A5" s="32" t="s">
+      <c r="A5" s="31" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="6" spans="1:1">
-      <c r="A6" s="32" t="s">
+      <c r="A6" s="31" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="7" spans="1:1">
-      <c r="A7" s="32" t="s">
+      <c r="A7" s="31" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="8" spans="1:1">
-      <c r="A8" s="32" t="s">
+      <c r="A8" s="31" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="9" spans="1:1">
-      <c r="A9" s="32" t="s">
+      <c r="A9" s="31" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="10" spans="1:1">
-      <c r="A10" s="32" t="s">
+      <c r="A10" s="31" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="11" spans="1:1">
-      <c r="A11" s="32" t="s">
+      <c r="A11" s="31" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="12" spans="1:1">
-      <c r="A12" s="32" t="s">
+      <c r="A12" s="31" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="13" spans="1:1">
-      <c r="A13" s="32" t="s">
+      <c r="A13" s="31" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="14" spans="1:1">
-      <c r="A14" s="32" t="s">
+      <c r="A14" s="31" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="15" spans="1:1">
-      <c r="A15" s="32" t="s">
+      <c r="A15" s="31" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="16" spans="1:1">
-      <c r="A16" s="32" t="s">
+      <c r="A16" s="31" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="17" spans="1:2">
-      <c r="A17" s="32" t="s">
+      <c r="A17" s="31" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="18" spans="1:2">
-      <c r="A18" s="32" t="s">
+      <c r="A18" s="31" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="19" spans="1:2">
-      <c r="A19" s="32" t="s">
+      <c r="A19" s="31" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="20" spans="1:2">
-      <c r="A20" s="32" t="s">
+      <c r="A20" s="31" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="21" spans="1:2">
-      <c r="A21" s="32" t="s">
+      <c r="A21" s="31" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="22" spans="1:2">
-      <c r="A22" s="32" t="s">
+      <c r="A22" s="31" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="23" spans="1:2">
-      <c r="A23" s="32" t="s">
+      <c r="A23" s="31" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="24" spans="1:2">
-      <c r="A24" s="32" t="s">
+      <c r="A24" s="31" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="25" spans="1:2">
-      <c r="A25" s="32" t="s">
+      <c r="A25" s="31" t="s">
         <v>29</v>
       </c>
-      <c r="B25" s="32">
+      <c r="B25" s="31">
         <v>43763</v>
       </c>
     </row>
     <row r="26" spans="1:2">
-      <c r="A26" s="32" t="s">
+      <c r="A26" s="31" t="s">
         <v>30</v>
       </c>
-      <c r="B26" s="32">
+      <c r="B26" s="31">
         <v>43756</v>
       </c>
     </row>
     <row r="27" spans="1:2">
-      <c r="A27" s="32" t="s">
+      <c r="A27" s="31" t="s">
         <v>31</v>
       </c>
-      <c r="B27" s="32">
+      <c r="B27" s="31">
         <v>43749</v>
       </c>
     </row>
     <row r="28" spans="1:2">
-      <c r="A28" s="32" t="s">
+      <c r="A28" s="31" t="s">
         <v>32</v>
       </c>
-      <c r="B28" s="32">
+      <c r="B28" s="31">
         <v>43742</v>
       </c>
     </row>
     <row r="29" spans="1:2">
-      <c r="A29" s="32" t="s">
+      <c r="A29" s="31" t="s">
         <v>33</v>
       </c>
-      <c r="B29" s="32">
+      <c r="B29" s="31">
         <v>43735</v>
       </c>
     </row>
     <row r="30" spans="1:2">
-      <c r="A30" s="32" t="s">
+      <c r="A30" s="31" t="s">
         <v>34</v>
       </c>
-      <c r="B30" s="32">
+      <c r="B30" s="31">
         <v>43728</v>
       </c>
     </row>
     <row r="31" spans="1:2">
-      <c r="A31" s="32" t="s">
+      <c r="A31" s="31" t="s">
         <v>35</v>
       </c>
-      <c r="B31" s="32">
+      <c r="B31" s="31">
         <v>43721</v>
       </c>
     </row>
     <row r="32" spans="1:2">
-      <c r="A32" s="32" t="s">
+      <c r="A32" s="31" t="s">
         <v>36</v>
       </c>
-      <c r="B32" s="32">
+      <c r="B32" s="31">
         <v>43714</v>
       </c>
     </row>
     <row r="33" spans="1:2">
-      <c r="A33" s="32" t="s">
+      <c r="A33" s="31" t="s">
         <v>37</v>
       </c>
-      <c r="B33" s="32">
+      <c r="B33" s="31">
         <v>43672</v>
       </c>
     </row>
     <row r="34" spans="1:2">
-      <c r="A34" s="32" t="s">
+      <c r="A34" s="31" t="s">
         <v>38</v>
       </c>
-      <c r="B34" s="32">
+      <c r="B34" s="31">
         <v>43665</v>
       </c>
     </row>
     <row r="35" spans="1:2">
-      <c r="A35" s="32" t="s">
+      <c r="A35" s="31" t="s">
         <v>39</v>
       </c>
-      <c r="B35" s="32">
+      <c r="B35" s="31">
         <v>43658</v>
       </c>
     </row>
     <row r="36" spans="1:2">
-      <c r="A36" s="32" t="s">
+      <c r="A36" s="31" t="s">
         <v>40</v>
       </c>
-      <c r="B36" s="32">
+      <c r="B36" s="31">
         <v>43651</v>
       </c>
     </row>
@@ -3611,17 +3651,13 @@
   <sheetPr codeName="Plan5"/>
   <dimension ref="A1:AC36"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E1" sqref="E1"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="10.7109375" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="26.28515625" style="19" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="10.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="29" width="9.140625" style="1" customWidth="1"/>
-    <col min="30" max="33" width="9.140625" style="31" customWidth="1"/>
-    <col min="34" max="16384" width="9.140625" style="31"/>
+    <col min="1" max="1" width="24.5703125" style="19" bestFit="1" customWidth="1"/>
+    <col min="2" max="29" width="10.7109375" style="1"/>
+    <col min="30" max="16384" width="10.7109375" style="30"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:29" s="20" customFormat="1" ht="26.25" customHeight="1">
@@ -3658,195 +3694,195 @@
       <c r="AC1" s="21"/>
     </row>
     <row r="2" spans="1:29">
-      <c r="A2" s="32" t="s">
+      <c r="A2" s="31" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="3" spans="1:29">
-      <c r="A3" s="32" t="s">
+      <c r="A3" s="31" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="4" spans="1:29">
-      <c r="A4" s="32" t="s">
+      <c r="A4" s="31" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="5" spans="1:29">
-      <c r="A5" s="32" t="s">
+      <c r="A5" s="31" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="6" spans="1:29">
-      <c r="A6" s="32" t="s">
+      <c r="A6" s="31" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="7" spans="1:29">
-      <c r="A7" s="32" t="s">
+      <c r="A7" s="31" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="8" spans="1:29">
-      <c r="A8" s="32" t="s">
+      <c r="A8" s="31" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="9" spans="1:29">
-      <c r="A9" s="32" t="s">
+      <c r="A9" s="31" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="10" spans="1:29">
-      <c r="A10" s="32" t="s">
+      <c r="A10" s="31" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="11" spans="1:29">
-      <c r="A11" s="32" t="s">
+      <c r="A11" s="31" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="12" spans="1:29">
-      <c r="A12" s="32" t="s">
+      <c r="A12" s="31" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="13" spans="1:29">
-      <c r="A13" s="32" t="s">
+      <c r="A13" s="31" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="14" spans="1:29">
-      <c r="A14" s="32" t="s">
+      <c r="A14" s="31" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="15" spans="1:29">
-      <c r="A15" s="32" t="s">
+      <c r="A15" s="31" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="16" spans="1:29">
-      <c r="A16" s="32" t="s">
+      <c r="A16" s="31" t="s">
         <v>20</v>
       </c>
-      <c r="B16" s="32" t="s">
+      <c r="B16" s="31" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="17" spans="1:2">
-      <c r="A17" s="32" t="s">
+      <c r="A17" s="31" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="18" spans="1:2">
-      <c r="A18" s="32" t="s">
+      <c r="A18" s="31" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="19" spans="1:2">
-      <c r="A19" s="32" t="s">
+      <c r="A19" s="31" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="20" spans="1:2">
-      <c r="A20" s="32" t="s">
+      <c r="A20" s="31" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="21" spans="1:2">
-      <c r="A21" s="32" t="s">
+      <c r="A21" s="31" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="22" spans="1:2">
-      <c r="A22" s="32" t="s">
+      <c r="A22" s="31" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="23" spans="1:2">
-      <c r="A23" s="32" t="s">
+      <c r="A23" s="31" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="24" spans="1:2">
-      <c r="A24" s="32" t="s">
+      <c r="A24" s="31" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="25" spans="1:2">
-      <c r="A25" s="32" t="s">
+      <c r="A25" s="31" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="26" spans="1:2">
-      <c r="A26" s="32" t="s">
+      <c r="A26" s="31" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="27" spans="1:2">
-      <c r="A27" s="32" t="s">
+      <c r="A27" s="31" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="28" spans="1:2">
-      <c r="A28" s="32" t="s">
+      <c r="A28" s="31" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="29" spans="1:2">
-      <c r="A29" s="32" t="s">
+      <c r="A29" s="31" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="30" spans="1:2">
-      <c r="A30" s="32" t="s">
+      <c r="A30" s="31" t="s">
         <v>34</v>
       </c>
-      <c r="B30" s="32">
+      <c r="B30" s="31">
         <v>43702</v>
       </c>
     </row>
     <row r="31" spans="1:2">
-      <c r="A31" s="32" t="s">
+      <c r="A31" s="31" t="s">
         <v>35</v>
       </c>
-      <c r="B31" s="32">
+      <c r="B31" s="31">
         <v>43701</v>
       </c>
     </row>
     <row r="32" spans="1:2">
-      <c r="A32" s="32" t="s">
+      <c r="A32" s="31" t="s">
         <v>36</v>
       </c>
-      <c r="B32" s="32">
+      <c r="B32" s="31">
         <v>43641</v>
       </c>
     </row>
     <row r="33" spans="1:2">
-      <c r="A33" s="32" t="s">
+      <c r="A33" s="31" t="s">
         <v>37</v>
       </c>
-      <c r="B33" s="32">
+      <c r="B33" s="31">
         <v>43703</v>
       </c>
     </row>
     <row r="34" spans="1:2">
-      <c r="A34" s="32" t="s">
+      <c r="A34" s="31" t="s">
         <v>38</v>
       </c>
-      <c r="B34" s="32">
+      <c r="B34" s="31">
         <v>43642</v>
       </c>
     </row>
     <row r="35" spans="1:2">
-      <c r="A35" s="32" t="s">
+      <c r="A35" s="31" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="36" spans="1:2">
-      <c r="A36" s="32" t="s">
+      <c r="A36" s="31" t="s">
         <v>40</v>
       </c>
     </row>
@@ -3857,564 +3893,563 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr codeName="Plan6"/>
   <dimension ref="A1:D49"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E1" sqref="E1"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="15" style="31" customWidth="1"/>
-    <col min="2" max="2" width="20" style="31" customWidth="1"/>
-    <col min="3" max="3" width="28" style="31" customWidth="1"/>
-    <col min="4" max="4" width="22" style="31" customWidth="1"/>
+    <col min="1" max="1" width="15" style="30" customWidth="1"/>
+    <col min="2" max="2" width="20" style="30" customWidth="1"/>
+    <col min="3" max="3" width="28" style="30" customWidth="1"/>
+    <col min="4" max="4" width="22" style="30" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="19.5">
-      <c r="A1" s="44" t="s">
+      <c r="A1" s="45" t="s">
         <v>47</v>
       </c>
-      <c r="B1" s="45"/>
-      <c r="C1" s="45"/>
-      <c r="D1" s="45"/>
+      <c r="B1" s="46"/>
+      <c r="C1" s="46"/>
+      <c r="D1" s="46"/>
     </row>
     <row r="2" spans="1:4">
-      <c r="A2" s="33"/>
-      <c r="B2" s="33"/>
-      <c r="C2" s="33"/>
-      <c r="D2" s="33"/>
+      <c r="A2" s="32"/>
+      <c r="B2" s="32"/>
+      <c r="C2" s="32"/>
+      <c r="D2" s="32"/>
     </row>
     <row r="3" spans="1:4">
-      <c r="A3" s="34" t="s">
+      <c r="A3" s="33" t="s">
         <v>48</v>
       </c>
-      <c r="B3" s="34" t="s">
+      <c r="B3" s="33" t="s">
         <v>49</v>
       </c>
-      <c r="C3" s="34" t="s">
+      <c r="C3" s="33" t="s">
         <v>50</v>
       </c>
-      <c r="D3" s="34" t="s">
+      <c r="D3" s="33" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="4" spans="1:4">
-      <c r="A4" s="34" t="s">
+      <c r="A4" s="33" t="s">
         <v>52</v>
       </c>
-      <c r="B4" s="34" t="s">
+      <c r="B4" s="33" t="s">
         <v>53</v>
       </c>
-      <c r="C4" s="34" t="s">
+      <c r="C4" s="33" t="s">
         <v>39</v>
       </c>
-      <c r="D4" s="34"/>
+      <c r="D4" s="33"/>
     </row>
     <row r="5" spans="1:4">
-      <c r="A5" s="34" t="s">
+      <c r="A5" s="33" t="s">
         <v>54</v>
       </c>
-      <c r="B5" s="34" t="s">
+      <c r="B5" s="33" t="s">
         <v>55</v>
       </c>
-      <c r="C5" s="34" t="s">
+      <c r="C5" s="33" t="s">
         <v>38</v>
       </c>
-      <c r="D5" s="34"/>
+      <c r="D5" s="33"/>
     </row>
     <row r="6" spans="1:4">
-      <c r="A6" s="34" t="s">
+      <c r="A6" s="33" t="s">
         <v>56</v>
       </c>
-      <c r="B6" s="34" t="s">
+      <c r="B6" s="33" t="s">
         <v>57</v>
       </c>
-      <c r="C6" s="34" t="s">
+      <c r="C6" s="33" t="s">
         <v>37</v>
       </c>
-      <c r="D6" s="34"/>
+      <c r="D6" s="33"/>
     </row>
     <row r="7" spans="1:4">
-      <c r="A7" s="35" t="s">
+      <c r="A7" s="34" t="s">
         <v>58</v>
       </c>
-      <c r="B7" s="35" t="s">
+      <c r="B7" s="34" t="s">
         <v>59</v>
       </c>
-      <c r="C7" s="35" t="s">
+      <c r="C7" s="34" t="s">
         <v>32</v>
       </c>
-      <c r="D7" s="34"/>
+      <c r="D7" s="33"/>
     </row>
     <row r="8" spans="1:4">
-      <c r="A8" s="36" t="s">
+      <c r="A8" s="35" t="s">
         <v>60</v>
       </c>
-      <c r="B8" s="36" t="s">
+      <c r="B8" s="35" t="s">
         <v>61</v>
       </c>
-      <c r="C8" s="36" t="s">
+      <c r="C8" s="35" t="s">
         <v>14</v>
       </c>
-      <c r="D8" s="34"/>
+      <c r="D8" s="33"/>
     </row>
     <row r="9" spans="1:4">
-      <c r="A9" s="36" t="s">
+      <c r="A9" s="35" t="s">
         <v>62</v>
       </c>
-      <c r="B9" s="36" t="s">
+      <c r="B9" s="35" t="s">
         <v>63</v>
       </c>
-      <c r="C9" s="36" t="s">
+      <c r="C9" s="35" t="s">
         <v>42</v>
       </c>
-      <c r="D9" s="34"/>
+      <c r="D9" s="33"/>
     </row>
     <row r="10" spans="1:4">
-      <c r="A10" s="34" t="s">
+      <c r="A10" s="33" t="s">
         <v>64</v>
       </c>
-      <c r="B10" s="34" t="s">
+      <c r="B10" s="33" t="s">
         <v>65</v>
       </c>
-      <c r="C10" s="34" t="s">
+      <c r="C10" s="33" t="s">
         <v>36</v>
       </c>
-      <c r="D10" s="34"/>
+      <c r="D10" s="33"/>
     </row>
     <row r="11" spans="1:4">
-      <c r="A11" s="34" t="s">
+      <c r="A11" s="33" t="s">
         <v>66</v>
       </c>
-      <c r="B11" s="34" t="s">
+      <c r="B11" s="33" t="s">
         <v>53</v>
       </c>
-      <c r="C11" s="34" t="s">
+      <c r="C11" s="33" t="s">
         <v>35</v>
       </c>
-      <c r="D11" s="34"/>
+      <c r="D11" s="33"/>
     </row>
     <row r="12" spans="1:4">
-      <c r="A12" s="34" t="s">
+      <c r="A12" s="33" t="s">
         <v>67</v>
       </c>
-      <c r="B12" s="34" t="s">
+      <c r="B12" s="33" t="s">
         <v>55</v>
       </c>
-      <c r="C12" s="34" t="s">
+      <c r="C12" s="33" t="s">
         <v>34</v>
       </c>
-      <c r="D12" s="34"/>
+      <c r="D12" s="33"/>
     </row>
     <row r="13" spans="1:4">
-      <c r="A13" s="34" t="s">
+      <c r="A13" s="33" t="s">
         <v>68</v>
       </c>
-      <c r="B13" s="34" t="s">
+      <c r="B13" s="33" t="s">
         <v>57</v>
       </c>
-      <c r="C13" s="34" t="s">
+      <c r="C13" s="33" t="s">
         <v>33</v>
       </c>
-      <c r="D13" s="34"/>
+      <c r="D13" s="33"/>
     </row>
     <row r="14" spans="1:4">
-      <c r="A14" s="35" t="s">
+      <c r="A14" s="34" t="s">
         <v>69</v>
       </c>
-      <c r="B14" s="35" t="s">
+      <c r="B14" s="34" t="s">
         <v>59</v>
       </c>
-      <c r="C14" s="35" t="s">
+      <c r="C14" s="34" t="s">
         <v>31</v>
       </c>
-      <c r="D14" s="34"/>
+      <c r="D14" s="33"/>
     </row>
     <row r="15" spans="1:4">
-      <c r="A15" s="36" t="s">
+      <c r="A15" s="35" t="s">
         <v>70</v>
       </c>
-      <c r="B15" s="36" t="s">
+      <c r="B15" s="35" t="s">
         <v>61</v>
       </c>
-      <c r="C15" s="36" t="s">
+      <c r="C15" s="35" t="s">
         <v>12</v>
       </c>
-      <c r="D15" s="34"/>
+      <c r="D15" s="33"/>
     </row>
     <row r="16" spans="1:4">
-      <c r="A16" s="36" t="s">
+      <c r="A16" s="35" t="s">
         <v>71</v>
       </c>
-      <c r="B16" s="36" t="s">
+      <c r="B16" s="35" t="s">
         <v>63</v>
       </c>
-      <c r="C16" s="36" t="s">
+      <c r="C16" s="35" t="s">
         <v>11</v>
       </c>
-      <c r="D16" s="34"/>
+      <c r="D16" s="33"/>
     </row>
     <row r="17" spans="1:4">
-      <c r="A17" s="36" t="s">
+      <c r="A17" s="35" t="s">
         <v>72</v>
       </c>
-      <c r="B17" s="36" t="s">
+      <c r="B17" s="35" t="s">
         <v>65</v>
       </c>
-      <c r="C17" s="36" t="s">
+      <c r="C17" s="35" t="s">
         <v>6</v>
       </c>
-      <c r="D17" s="34"/>
+      <c r="D17" s="33"/>
     </row>
     <row r="18" spans="1:4">
-      <c r="A18" s="34" t="s">
+      <c r="A18" s="33" t="s">
         <v>73</v>
       </c>
-      <c r="B18" s="34" t="s">
+      <c r="B18" s="33" t="s">
         <v>53</v>
       </c>
-      <c r="C18" s="34" t="s">
+      <c r="C18" s="33" t="s">
         <v>31</v>
       </c>
-      <c r="D18" s="34"/>
+      <c r="D18" s="33"/>
     </row>
     <row r="19" spans="1:4">
-      <c r="A19" s="34" t="s">
+      <c r="A19" s="33" t="s">
         <v>74</v>
       </c>
-      <c r="B19" s="34" t="s">
+      <c r="B19" s="33" t="s">
         <v>55</v>
       </c>
-      <c r="C19" s="34" t="s">
+      <c r="C19" s="33" t="s">
         <v>29</v>
       </c>
-      <c r="D19" s="34"/>
+      <c r="D19" s="33"/>
     </row>
     <row r="20" spans="1:4">
-      <c r="A20" s="34" t="s">
+      <c r="A20" s="33" t="s">
         <v>75</v>
       </c>
-      <c r="B20" s="34" t="s">
+      <c r="B20" s="33" t="s">
         <v>57</v>
       </c>
-      <c r="C20" s="34" t="s">
+      <c r="C20" s="33" t="s">
         <v>28</v>
       </c>
-      <c r="D20" s="34"/>
+      <c r="D20" s="33"/>
     </row>
     <row r="21" spans="1:4">
-      <c r="A21" s="35" t="s">
+      <c r="A21" s="34" t="s">
         <v>76</v>
       </c>
-      <c r="B21" s="35" t="s">
+      <c r="B21" s="34" t="s">
         <v>59</v>
       </c>
-      <c r="C21" s="35" t="s">
+      <c r="C21" s="34" t="s">
         <v>30</v>
       </c>
-      <c r="D21" s="34"/>
+      <c r="D21" s="33"/>
     </row>
     <row r="22" spans="1:4">
-      <c r="A22" s="36" t="s">
+      <c r="A22" s="35" t="s">
         <v>77</v>
       </c>
-      <c r="B22" s="36" t="s">
+      <c r="B22" s="35" t="s">
         <v>61</v>
       </c>
-      <c r="C22" s="36" t="s">
+      <c r="C22" s="35" t="s">
         <v>10</v>
       </c>
-      <c r="D22" s="34"/>
+      <c r="D22" s="33"/>
     </row>
     <row r="23" spans="1:4">
-      <c r="A23" s="36" t="s">
+      <c r="A23" s="35" t="s">
         <v>78</v>
       </c>
-      <c r="B23" s="36" t="s">
+      <c r="B23" s="35" t="s">
         <v>63</v>
       </c>
-      <c r="C23" s="36" t="s">
+      <c r="C23" s="35" t="s">
         <v>9</v>
       </c>
-      <c r="D23" s="34"/>
+      <c r="D23" s="33"/>
     </row>
     <row r="24" spans="1:4">
-      <c r="A24" s="34" t="s">
+      <c r="A24" s="33" t="s">
         <v>79</v>
       </c>
-      <c r="B24" s="34" t="s">
+      <c r="B24" s="33" t="s">
         <v>65</v>
       </c>
-      <c r="C24" s="34" t="s">
+      <c r="C24" s="33" t="s">
         <v>30</v>
       </c>
-      <c r="D24" s="34"/>
+      <c r="D24" s="33"/>
     </row>
     <row r="25" spans="1:4">
-      <c r="A25" s="36" t="s">
+      <c r="A25" s="35" t="s">
         <v>80</v>
       </c>
-      <c r="B25" s="36" t="s">
+      <c r="B25" s="35" t="s">
         <v>53</v>
       </c>
-      <c r="C25" s="36" t="s">
+      <c r="C25" s="35" t="s">
         <v>40</v>
       </c>
-      <c r="D25" s="34"/>
+      <c r="D25" s="33"/>
     </row>
     <row r="26" spans="1:4">
-      <c r="A26" s="34" t="s">
+      <c r="A26" s="33" t="s">
         <v>81</v>
       </c>
-      <c r="B26" s="34" t="s">
+      <c r="B26" s="33" t="s">
         <v>55</v>
       </c>
-      <c r="C26" s="34" t="s">
+      <c r="C26" s="33" t="s">
         <v>26</v>
       </c>
-      <c r="D26" s="34"/>
+      <c r="D26" s="33"/>
     </row>
     <row r="27" spans="1:4">
-      <c r="A27" s="34" t="s">
+      <c r="A27" s="33" t="s">
         <v>82</v>
       </c>
-      <c r="B27" s="34" t="s">
+      <c r="B27" s="33" t="s">
         <v>57</v>
       </c>
-      <c r="C27" s="34" t="s">
+      <c r="C27" s="33" t="s">
         <v>25</v>
       </c>
-      <c r="D27" s="34"/>
+      <c r="D27" s="33"/>
     </row>
     <row r="28" spans="1:4">
-      <c r="A28" s="35" t="s">
+      <c r="A28" s="34" t="s">
         <v>83</v>
       </c>
-      <c r="B28" s="35" t="s">
+      <c r="B28" s="34" t="s">
         <v>59</v>
       </c>
-      <c r="C28" s="35" t="s">
+      <c r="C28" s="34" t="s">
         <v>29</v>
       </c>
-      <c r="D28" s="34"/>
+      <c r="D28" s="33"/>
     </row>
     <row r="29" spans="1:4">
-      <c r="A29" s="36" t="s">
+      <c r="A29" s="35" t="s">
         <v>84</v>
       </c>
-      <c r="B29" s="36" t="s">
+      <c r="B29" s="35" t="s">
         <v>61</v>
       </c>
-      <c r="C29" s="36" t="s">
+      <c r="C29" s="35" t="s">
         <v>8</v>
       </c>
-      <c r="D29" s="34"/>
+      <c r="D29" s="33"/>
     </row>
     <row r="30" spans="1:4">
-      <c r="A30" s="36" t="s">
+      <c r="A30" s="35" t="s">
         <v>85</v>
       </c>
-      <c r="B30" s="36" t="s">
+      <c r="B30" s="35" t="s">
         <v>63</v>
       </c>
-      <c r="C30" s="36" t="s">
+      <c r="C30" s="35" t="s">
         <v>7</v>
       </c>
-      <c r="D30" s="34"/>
+      <c r="D30" s="33"/>
     </row>
     <row r="31" spans="1:4">
-      <c r="A31" s="34" t="s">
+      <c r="A31" s="33" t="s">
         <v>86</v>
       </c>
-      <c r="B31" s="34" t="s">
+      <c r="B31" s="33" t="s">
         <v>65</v>
       </c>
-      <c r="C31" s="34" t="s">
+      <c r="C31" s="33" t="s">
         <v>24</v>
       </c>
-      <c r="D31" s="34"/>
+      <c r="D31" s="33"/>
     </row>
     <row r="32" spans="1:4">
-      <c r="A32" s="34" t="s">
+      <c r="A32" s="33" t="s">
         <v>87</v>
       </c>
-      <c r="B32" s="34" t="s">
+      <c r="B32" s="33" t="s">
         <v>53</v>
       </c>
-      <c r="C32" s="34" t="s">
+      <c r="C32" s="33" t="s">
         <v>23</v>
       </c>
-      <c r="D32" s="34"/>
+      <c r="D32" s="33"/>
     </row>
     <row r="33" spans="1:4">
-      <c r="A33" s="36" t="s">
+      <c r="A33" s="35" t="s">
         <v>88</v>
       </c>
-      <c r="B33" s="36" t="s">
+      <c r="B33" s="35" t="s">
         <v>55</v>
       </c>
-      <c r="C33" s="36" t="s">
+      <c r="C33" s="35" t="s">
         <v>39</v>
       </c>
-      <c r="D33" s="34"/>
+      <c r="D33" s="33"/>
     </row>
     <row r="34" spans="1:4">
-      <c r="A34" s="34" t="s">
+      <c r="A34" s="33" t="s">
         <v>89</v>
       </c>
-      <c r="B34" s="34" t="s">
+      <c r="B34" s="33" t="s">
         <v>57</v>
       </c>
-      <c r="C34" s="34" t="s">
+      <c r="C34" s="33" t="s">
         <v>21</v>
       </c>
-      <c r="D34" s="34"/>
+      <c r="D34" s="33"/>
     </row>
     <row r="36" spans="1:4">
-      <c r="C36" s="37"/>
+      <c r="C36" s="36"/>
     </row>
     <row r="37" spans="1:4">
-      <c r="A37" s="40" t="s">
+      <c r="A37" s="41" t="s">
         <v>90</v>
       </c>
-      <c r="B37" s="41"/>
-      <c r="C37" s="41"/>
-      <c r="D37" s="42"/>
+      <c r="B37" s="42"/>
+      <c r="C37" s="42"/>
+      <c r="D37" s="43"/>
     </row>
     <row r="38" spans="1:4">
-      <c r="A38" s="43" t="s">
+      <c r="A38" s="44" t="s">
         <v>41</v>
       </c>
-      <c r="B38" s="42"/>
-      <c r="C38" s="35" t="s">
+      <c r="B38" s="43"/>
+      <c r="C38" s="34" t="s">
         <v>45</v>
       </c>
-      <c r="D38" s="34" t="s">
+      <c r="D38" s="33" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="39" spans="1:4">
-      <c r="A39" s="36" t="s">
+      <c r="A39" s="35" t="s">
         <v>60</v>
       </c>
-      <c r="B39" s="36" t="s">
+      <c r="B39" s="35" t="s">
         <v>38</v>
       </c>
-      <c r="C39" s="35" t="s">
+      <c r="C39" s="34" t="s">
         <v>28</v>
       </c>
-      <c r="D39" s="34" t="s">
+      <c r="D39" s="33" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="40" spans="1:4">
-      <c r="A40" s="36" t="s">
+      <c r="A40" s="35" t="s">
         <v>62</v>
       </c>
-      <c r="B40" s="36" t="s">
+      <c r="B40" s="35" t="s">
         <v>37</v>
       </c>
-      <c r="C40" s="35" t="s">
+      <c r="C40" s="34" t="s">
         <v>27</v>
       </c>
-      <c r="D40" s="34" t="s">
+      <c r="D40" s="33" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="41" spans="1:4">
-      <c r="A41" s="36" t="s">
+      <c r="A41" s="35" t="s">
         <v>70</v>
       </c>
-      <c r="B41" s="36" t="s">
+      <c r="B41" s="35" t="s">
         <v>36</v>
       </c>
-      <c r="C41" s="35" t="s">
+      <c r="C41" s="34" t="s">
         <v>26</v>
       </c>
-      <c r="D41" s="34" t="s">
+      <c r="D41" s="33" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="42" spans="1:4">
-      <c r="A42" s="36" t="s">
+      <c r="A42" s="35" t="s">
         <v>71</v>
       </c>
-      <c r="B42" s="36" t="s">
+      <c r="B42" s="35" t="s">
         <v>35</v>
       </c>
-      <c r="C42" s="37"/>
+      <c r="C42" s="36"/>
       <c r="D42"/>
     </row>
     <row r="43" spans="1:4">
-      <c r="A43" s="36" t="s">
+      <c r="A43" s="35" t="s">
         <v>72</v>
       </c>
-      <c r="B43" s="36" t="s">
+      <c r="B43" s="35" t="s">
         <v>34</v>
       </c>
-      <c r="C43" s="37"/>
+      <c r="C43" s="36"/>
       <c r="D43"/>
     </row>
     <row r="44" spans="1:4">
-      <c r="A44" s="36" t="s">
+      <c r="A44" s="35" t="s">
         <v>77</v>
       </c>
-      <c r="B44" s="36" t="s">
+      <c r="B44" s="35" t="s">
         <v>33</v>
       </c>
-      <c r="C44" s="37"/>
+      <c r="C44" s="36"/>
       <c r="D44"/>
     </row>
     <row r="45" spans="1:4">
-      <c r="A45" s="36" t="s">
+      <c r="A45" s="35" t="s">
         <v>78</v>
       </c>
-      <c r="B45" s="36" t="s">
+      <c r="B45" s="35" t="s">
         <v>32</v>
       </c>
-      <c r="C45" s="37"/>
+      <c r="C45" s="36"/>
       <c r="D45"/>
     </row>
     <row r="46" spans="1:4">
-      <c r="A46" s="36" t="s">
+      <c r="A46" s="35" t="s">
         <v>80</v>
       </c>
-      <c r="B46" s="36" t="s">
+      <c r="B46" s="35" t="s">
         <v>31</v>
       </c>
-      <c r="C46" s="37"/>
+      <c r="C46" s="36"/>
       <c r="D46"/>
     </row>
     <row r="47" spans="1:4">
-      <c r="A47" s="36" t="s">
+      <c r="A47" s="35" t="s">
         <v>84</v>
       </c>
-      <c r="B47" s="36" t="s">
+      <c r="B47" s="35" t="s">
         <v>30</v>
       </c>
-      <c r="C47" s="37"/>
+      <c r="C47" s="36"/>
       <c r="D47"/>
     </row>
     <row r="48" spans="1:4">
-      <c r="A48" s="36" t="s">
+      <c r="A48" s="35" t="s">
         <v>85</v>
       </c>
-      <c r="B48" s="36" t="s">
+      <c r="B48" s="35" t="s">
         <v>28</v>
       </c>
-      <c r="C48" s="37"/>
+      <c r="C48" s="36"/>
       <c r="D48"/>
     </row>
     <row r="49" spans="1:4">
-      <c r="A49" s="36" t="s">
+      <c r="A49" s="35" t="s">
         <v>88</v>
       </c>
-      <c r="B49" s="36" t="s">
+      <c r="B49" s="35" t="s">
         <v>27</v>
       </c>
-      <c r="C49" s="37"/>
+      <c r="C49" s="36"/>
       <c r="D49"/>
     </row>
   </sheetData>
@@ -4423,6 +4458,7 @@
     <mergeCell ref="A38:B38"/>
     <mergeCell ref="A1:D1"/>
   </mergeCells>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>